<commit_message>
Subsetting data from roils .xlsx functional
</commit_message>
<xml_diff>
--- a/TQA/extracted.xlsx
+++ b/TQA/extracted.xlsx
@@ -445,27 +445,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10X.Date_Time_Submitted</t>
+          <t>Date_Time_Submitted</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>104.Classification</t>
+          <t>Classification</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>102.Location_Sub</t>
+          <t>Location_Sub</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>105.Narrative</t>
+          <t>Narrative</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>106.Tx_Technique</t>
+          <t>Tx_Technique</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -475,22 +475,22 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>108.Reporter_Name</t>
+          <t>Reporter_Name</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>202.Discoverer_Role</t>
+          <t>Discoverer_Role</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>205.Narrative_Supplemental</t>
+          <t>Narrative_Supplemental</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>201.Event_Title</t>
+          <t>Event_Title</t>
         </is>
       </c>
     </row>

</xml_diff>